<commit_message>
Suite plan de financement
</commit_message>
<xml_diff>
--- a/Plan de financement.xlsx
+++ b/Plan de financement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/damiencollot/Documents/git/Repart/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A4146F0-8544-DC41-8180-47A911BC7C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1DF620-800C-5143-99A7-B503C4D1FA4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{BCB8DCC3-E3B3-8C41-AA6D-481C9FDFAB40}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{BCB8DCC3-E3B3-8C41-AA6D-481C9FDFAB40}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -32,12 +32,127 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+  <si>
+    <t>Coût Humain</t>
+  </si>
+  <si>
+    <t>Nicolas</t>
+  </si>
+  <si>
+    <t>Ayman</t>
+  </si>
+  <si>
+    <t>Damien</t>
+  </si>
+  <si>
+    <t>Mathieu</t>
+  </si>
+  <si>
+    <t>Prénom</t>
+  </si>
+  <si>
+    <t>Métier</t>
+  </si>
+  <si>
+    <t>Coût horaire</t>
+  </si>
+  <si>
+    <t>Développeur</t>
+  </si>
+  <si>
+    <t>Consultant financier</t>
+  </si>
+  <si>
+    <t>Chef de Projet</t>
+  </si>
+  <si>
+    <t>Nombre d'heures travaillé</t>
+  </si>
+  <si>
+    <t>Coût total</t>
+  </si>
+  <si>
+    <t>Coût matériel</t>
+  </si>
+  <si>
+    <t>Bracelet connecté (Repart Tempo)</t>
+  </si>
+  <si>
+    <t>Serveur</t>
+  </si>
+  <si>
+    <t>Quantité</t>
+  </si>
+  <si>
+    <t>Cout individuel</t>
+  </si>
+  <si>
+    <t>Matériel</t>
+  </si>
+  <si>
+    <t>MacBook Pro 13"</t>
+  </si>
+  <si>
+    <t>Magnétophone connecté (Repart Listener)</t>
+  </si>
+  <si>
+    <t>Total :</t>
+  </si>
+  <si>
+    <t>Coût supplémentaire</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Coût</t>
+  </si>
+  <si>
+    <t>Livraison 4 Repart Tempo, 1 Repart Listener</t>
+  </si>
+  <si>
+    <t>Livraison 100 Repart Tempo, 1 Repart Listener</t>
+  </si>
+  <si>
+    <t>Livraison 1 Repart Listener</t>
+  </si>
+  <si>
+    <t>Location d'un serveur</t>
+  </si>
+  <si>
+    <t>95,99 par mois</t>
+  </si>
+  <si>
+    <t>Livraison 1 Repart Tempo, 1 Repart Listener</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="#,##0.00\ &quot;€&quot;"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -51,7 +166,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -59,12 +174,502 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFC00000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFC00000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFC00000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFC00000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFC00000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC00000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFC00000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC00000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFC00000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC00000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFC00000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC00000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFC00000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFC00000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFC00000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC00000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFC00000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC00000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFC00000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC00000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFC00000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC00000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFC00000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC00000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFC00000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFC00000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFC00000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC00000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFC00000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC00000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFC00000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFC00000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFC00000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC00000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFC00000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFC00000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFC00000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFC00000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFC00000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFC00000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFC00000"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FFC00000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFC00000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color rgb="FFC00000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFC00000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFC00000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFC00000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFC00000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="4"/>
+      </left>
+      <right style="thick">
+        <color theme="4"/>
+      </right>
+      <top style="thick">
+        <color theme="4"/>
+      </top>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thick">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thick">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thick">
+        <color theme="4"/>
+      </right>
+      <top style="thick">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thick">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thick">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF00B0F0"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF00B0F0"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF00B0F0"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF00B0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF00B0F0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF00B0F0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF00B0F0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF00B0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF00B0F0"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF00B0F0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF00B0F0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF00B0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF00B0F0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF00B0F0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF00B0F0"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF00B0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF00B0F0"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF00B0F0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF00B0F0"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF00B0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF00B0F0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF00B0F0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF00B0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF00B0F0"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF00B0F0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF00B0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,12 +984,273 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAFBEBCE-ECDD-F342-8B44-80E9D1DC0215}">
-  <dimension ref="A1"/>
+  <dimension ref="A3:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="30"/>
+      <c r="I4" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+    </row>
+    <row r="5" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="11">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1120</v>
+      </c>
+      <c r="E6" s="8">
+        <f>C6*D6</f>
+        <v>22400</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="15">
+        <v>8</v>
+      </c>
+      <c r="K6" s="16">
+        <v>50</v>
+      </c>
+      <c r="L6" s="17">
+        <f>J6*K6</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="12">
+        <v>20</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1120</v>
+      </c>
+      <c r="E7" s="9">
+        <f t="shared" ref="E7:E9" si="0">C7*D7</f>
+        <v>22400</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="19">
+        <v>2</v>
+      </c>
+      <c r="K7" s="20">
+        <v>300</v>
+      </c>
+      <c r="L7" s="21">
+        <f t="shared" ref="L7:L9" si="1">J7*K7</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="12">
+        <v>17.54</v>
+      </c>
+      <c r="D8" s="4">
+        <v>35</v>
+      </c>
+      <c r="E8" s="9">
+        <f t="shared" si="0"/>
+        <v>613.9</v>
+      </c>
+      <c r="I8" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="19">
+        <v>4</v>
+      </c>
+      <c r="K8" s="20">
+        <v>1599</v>
+      </c>
+      <c r="L8" s="21">
+        <f t="shared" si="1"/>
+        <v>6396</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="13">
+        <v>23</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1120</v>
+      </c>
+      <c r="E9" s="10">
+        <f t="shared" si="0"/>
+        <v>25760</v>
+      </c>
+      <c r="I9" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="23">
+        <v>1</v>
+      </c>
+      <c r="K9" s="24">
+        <v>300</v>
+      </c>
+      <c r="L9" s="25">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="7">
+        <f>SUM(E6:E9)</f>
+        <v>71173.899999999994</v>
+      </c>
+      <c r="K11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" s="7">
+        <f>SUM(L6:L9)</f>
+        <v>7696</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="39"/>
+      <c r="F15" s="32"/>
+    </row>
+    <row r="16" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D16" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="D17" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="38">
+        <v>6.55</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D18" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="34">
+        <v>14.1</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D19" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="34">
+        <v>7.45</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D20" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="34">
+        <v>4.95</v>
+      </c>
+    </row>
+    <row r="21" spans="4:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="36" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="4:5" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="D15:E15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fin plan de financement
</commit_message>
<xml_diff>
--- a/Plan de financement.xlsx
+++ b/Plan de financement.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/damiencollot/Documents/git/Repart/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1DF620-800C-5143-99A7-B503C4D1FA4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6DE48E9-8B6B-024D-A7F1-9F18A56E2E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{BCB8DCC3-E3B3-8C41-AA6D-481C9FDFAB40}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -133,7 +133,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -166,7 +166,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -310,21 +310,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFC00000"/>
-      </left>
-      <right style="thick">
-        <color rgb="FFC00000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFC00000"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FFC00000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thick">
         <color rgb="FFC00000"/>
       </left>
@@ -609,6 +594,92 @@
       <top/>
       <bottom style="thin">
         <color rgb="FF00B0F0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFC00000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC00000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFC00000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFC00000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFC00000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFC00000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFC00000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC00000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFC00000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFC00000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFC00000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFC00000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFC00000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFC00000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thick">
+        <color theme="4"/>
+      </top>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thick">
+        <color theme="4"/>
+      </right>
+      <top style="thick">
+        <color theme="4"/>
+      </top>
+      <bottom style="thick">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -616,7 +687,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -624,29 +695,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -656,20 +736,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -987,7 +1062,7 @@
   <dimension ref="A3:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1001,46 +1076,46 @@
   <sheetData>
     <row r="3" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="30"/>
-      <c r="I4" s="26" t="s">
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="36"/>
+      <c r="I4" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
     </row>
     <row r="5" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="27" t="s">
+      <c r="I5" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="27" t="s">
+      <c r="J5" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="27" t="s">
+      <c r="K5" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="27" t="s">
+      <c r="L5" s="24" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1051,28 +1126,28 @@
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="9">
         <v>20</v>
       </c>
       <c r="D6" s="2">
         <v>1120</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <f>C6*D6</f>
         <v>22400</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="15">
+      <c r="J6" s="13">
         <v>8</v>
       </c>
-      <c r="K6" s="16">
-        <v>50</v>
-      </c>
-      <c r="L6" s="17">
+      <c r="K6" s="14">
+        <v>100</v>
+      </c>
+      <c r="L6" s="15">
         <f>J6*K6</f>
-        <v>400</v>
+        <v>800</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -1082,28 +1157,28 @@
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="10">
         <v>20</v>
       </c>
       <c r="D7" s="4">
         <v>1120</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8">
         <f t="shared" ref="E7:E9" si="0">C7*D7</f>
         <v>22400</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="I7" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="19">
+      <c r="J7" s="17">
         <v>2</v>
       </c>
-      <c r="K7" s="20">
-        <v>300</v>
-      </c>
-      <c r="L7" s="21">
+      <c r="K7" s="18">
+        <v>500</v>
+      </c>
+      <c r="L7" s="19">
         <f t="shared" ref="L7:L9" si="1">J7*K7</f>
-        <v>600</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -1113,26 +1188,26 @@
       <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="10">
         <v>17.54</v>
       </c>
       <c r="D8" s="4">
         <v>35</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="8">
         <f t="shared" si="0"/>
         <v>613.9</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="I8" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="19">
+      <c r="J8" s="17">
         <v>4</v>
       </c>
-      <c r="K8" s="20">
+      <c r="K8" s="18">
         <v>1599</v>
       </c>
-      <c r="L8" s="21">
+      <c r="L8" s="19">
         <f t="shared" si="1"/>
         <v>6396</v>
       </c>
@@ -1144,103 +1219,100 @@
       <c r="B9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="11">
         <v>23</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="39">
         <v>1120</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="40">
         <f t="shared" si="0"/>
         <v>25760</v>
       </c>
-      <c r="I9" s="22" t="s">
+      <c r="I9" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="23">
+      <c r="J9" s="21">
         <v>1</v>
       </c>
-      <c r="K9" s="24">
+      <c r="K9" s="22">
         <v>300</v>
       </c>
-      <c r="L9" s="25">
+      <c r="L9" s="23">
         <f t="shared" si="1"/>
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D11" t="s">
+    <row r="10" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E10" s="42">
         <f>SUM(E6:E9)</f>
         <v>71173.899999999994</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K10" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="L11" s="7">
+      <c r="L10" s="44">
         <f>SUM(L6:L9)</f>
-        <v>7696</v>
+        <v>8496</v>
       </c>
     </row>
+    <row r="11" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="39" t="s">
+      <c r="D15" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="39"/>
-      <c r="F15" s="32"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="26"/>
     </row>
     <row r="16" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="40" t="s">
+      <c r="E16" s="33" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" spans="4:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="D17" s="37" t="s">
+      <c r="D17" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="38">
+      <c r="E17" s="32">
         <v>6.55</v>
       </c>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D18" s="33" t="s">
+      <c r="D18" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="34">
+      <c r="E18" s="28">
         <v>14.1</v>
       </c>
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="34">
+      <c r="E19" s="28">
         <v>7.45</v>
       </c>
     </row>
     <row r="20" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D20" s="33" t="s">
+      <c r="D20" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="34">
+      <c r="E20" s="28">
         <v>4.95</v>
       </c>
     </row>
     <row r="21" spans="4:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D21" s="35" t="s">
+      <c r="D21" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="36" t="s">
+      <c r="E21" s="30" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fin du projet repart
</commit_message>
<xml_diff>
--- a/Plan de financement.xlsx
+++ b/Plan de financement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/damiencollot/Documents/git/Repart/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6DE48E9-8B6B-024D-A7F1-9F18A56E2E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E396CBD-CC98-5A4A-8CB6-09632844F2E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{BCB8DCC3-E3B3-8C41-AA6D-481C9FDFAB40}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Coût Humain</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>Livraison 1 Repart Tempo, 1 Repart Listener</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coût total : </t>
   </si>
 </sst>
 </file>
@@ -166,7 +169,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -683,11 +686,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color theme="9"/>
+      </left>
+      <right style="thick">
+        <color theme="9"/>
+      </right>
+      <top style="thick">
+        <color theme="9"/>
+      </top>
+      <bottom style="thick">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -724,6 +742,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -739,12 +767,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1059,14 +1081,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAFBEBCE-ECDD-F342-8B44-80E9D1DC0215}">
-  <dimension ref="A3:L22"/>
+  <dimension ref="A3:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="39.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
@@ -1076,19 +1099,19 @@
   <sheetData>
     <row r="3" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="36"/>
-      <c r="I4" s="37" t="s">
+      <c r="B4" s="43"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="44"/>
+      <c r="I4" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
     </row>
     <row r="5" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
@@ -1127,14 +1150,14 @@
         <v>8</v>
       </c>
       <c r="C6" s="9">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="D6" s="2">
-        <v>1120</v>
+        <v>1400</v>
       </c>
       <c r="E6" s="7">
         <f>C6*D6</f>
-        <v>22400</v>
+        <v>60200</v>
       </c>
       <c r="I6" s="12" t="s">
         <v>14</v>
@@ -1158,14 +1181,14 @@
         <v>8</v>
       </c>
       <c r="C7" s="10">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="D7" s="4">
-        <v>1120</v>
+        <v>1400</v>
       </c>
       <c r="E7" s="8">
         <f t="shared" ref="E7:E9" si="0">C7*D7</f>
-        <v>22400</v>
+        <v>60200</v>
       </c>
       <c r="I7" s="16" t="s">
         <v>20</v>
@@ -1189,14 +1212,14 @@
         <v>9</v>
       </c>
       <c r="C8" s="10">
-        <v>17.54</v>
+        <v>43</v>
       </c>
       <c r="D8" s="4">
-        <v>35</v>
+        <v>1400</v>
       </c>
       <c r="E8" s="8">
         <f t="shared" si="0"/>
-        <v>613.9</v>
+        <v>60200</v>
       </c>
       <c r="I8" s="16" t="s">
         <v>19</v>
@@ -1220,14 +1243,14 @@
         <v>10</v>
       </c>
       <c r="C9" s="11">
-        <v>23</v>
-      </c>
-      <c r="D9" s="39">
-        <v>1120</v>
-      </c>
-      <c r="E9" s="40">
+        <v>43</v>
+      </c>
+      <c r="D9" s="34">
+        <v>1400</v>
+      </c>
+      <c r="E9" s="35">
         <f t="shared" si="0"/>
-        <v>25760</v>
+        <v>60200</v>
       </c>
       <c r="I9" s="20" t="s">
         <v>15</v>
@@ -1244,84 +1267,93 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="41" t="s">
+      <c r="D10" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="42">
+      <c r="E10" s="37">
         <f>SUM(E6:E9)</f>
-        <v>71173.899999999994</v>
-      </c>
-      <c r="K10" s="43" t="s">
+        <v>240800</v>
+      </c>
+      <c r="K10" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="L10" s="44">
+      <c r="L10" s="39">
         <f>SUM(L6:L9)</f>
         <v>8496</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="40">
+        <f>SUM(E10,L10)</f>
+        <v>249296</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="46"/>
+    </row>
     <row r="15" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="38"/>
+      <c r="A15" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>24</v>
+      </c>
       <c r="F15" s="26"/>
     </row>
-    <row r="16" spans="1:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D16" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="33" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="4:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="D17" s="31" t="s">
+    <row r="16" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="32">
+      <c r="B16" s="32">
         <v>6.55</v>
       </c>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D18" s="27" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="28">
+      <c r="B17" s="28">
         <v>14.1</v>
       </c>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D19" s="27" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="28">
+      <c r="B18" s="28">
         <v>7.45</v>
       </c>
     </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D20" s="27" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="28">
+      <c r="B19" s="28">
         <v>4.95</v>
       </c>
     </row>
-    <row r="21" spans="4:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D21" s="29" t="s">
+    <row r="20" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="30" t="s">
+      <c r="B20" s="30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="4:5" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="I4:L4"/>
-    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="A14:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>